<commit_message>
dev 1.0.0 : update templete rename mte2 to mte1
</commit_message>
<xml_diff>
--- a/public/files/TemplateCapexExport.xlsx
+++ b/public/files/TemplateCapexExport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\#AIIA\2023\improve system AIIA_Budget\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Project Management\01_Source code\new_cubic_pro\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B612D777-7B04-492E-8CC5-6597F3B74DD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F4AEB8-566A-4A11-ADF0-8AC07DA7A29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary CAPEX" sheetId="3" r:id="rId1"/>
@@ -24,6 +24,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -230,9 +241,6 @@
     <t>QAS3</t>
   </si>
   <si>
-    <t>MTE2</t>
-  </si>
-  <si>
     <t>ITD1</t>
   </si>
   <si>
@@ -274,16 +282,19 @@
   <si>
     <t>PPU</t>
   </si>
+  <si>
+    <t>MTE1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +313,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -373,14 +390,14 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="2" fillId="2" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -392,12 +409,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -407,23 +424,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Koma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Persen" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -703,7 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AT14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -2335,11 +2352,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:AW199"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="AN75" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="AH56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AL78" sqref="AL78:AW78"/>
+      <selection pane="bottomRight" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11066,7 +11083,7 @@
         <v>21</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>22</v>
@@ -11245,7 +11262,7 @@
         <v>21</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="7" t="s">
@@ -11388,7 +11405,7 @@
         <v>21</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="7" t="s">
@@ -11531,7 +11548,7 @@
         <v>21</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="7" t="s">
@@ -11674,7 +11691,7 @@
         <v>21</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="7" t="s">
@@ -11817,7 +11834,7 @@
         <v>21</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="7" t="s">
@@ -11960,7 +11977,7 @@
         <v>21</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="7" t="s">
@@ -12103,7 +12120,7 @@
         <v>21</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="7" t="s">
@@ -12246,7 +12263,7 @@
         <v>23</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>23</v>
@@ -12425,7 +12442,7 @@
         <v>23</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="7" t="s">
@@ -12568,7 +12585,7 @@
         <v>23</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C72" s="7"/>
       <c r="D72" s="7" t="s">
@@ -12711,7 +12728,7 @@
         <v>23</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="7" t="s">
@@ -12854,7 +12871,7 @@
         <v>23</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C74" s="7"/>
       <c r="D74" s="7" t="s">
@@ -12997,7 +13014,7 @@
         <v>23</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="7" t="s">
@@ -13140,7 +13157,7 @@
         <v>23</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C76" s="7"/>
       <c r="D76" s="7" t="s">
@@ -13283,7 +13300,7 @@
         <v>23</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="7" t="s">
@@ -13603,7 +13620,7 @@
         <v>26</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>27</v>
@@ -13619,11 +13636,11 @@
         <v>0</v>
       </c>
       <c r="H79" s="8">
-        <f t="shared" ref="H78:H79" si="172">SUBTOTAL(9,H80:H86)</f>
+        <f t="shared" ref="H79" si="172">SUBTOTAL(9,H80:H86)</f>
         <v>0</v>
       </c>
       <c r="I79" s="8">
-        <f t="shared" ref="I78:I79" si="173">SUBTOTAL(9,I80:I86)</f>
+        <f t="shared" ref="I79" si="173">SUBTOTAL(9,I80:I86)</f>
         <v>0</v>
       </c>
       <c r="J79" s="8">
@@ -13782,7 +13799,7 @@
         <v>26</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80" s="7" t="s">
@@ -13925,7 +13942,7 @@
         <v>26</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C81" s="7"/>
       <c r="D81" s="7" t="s">
@@ -14068,7 +14085,7 @@
         <v>26</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C82" s="7"/>
       <c r="D82" s="7" t="s">
@@ -14211,7 +14228,7 @@
         <v>26</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="7" t="s">
@@ -14354,7 +14371,7 @@
         <v>26</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C84" s="7"/>
       <c r="D84" s="7" t="s">
@@ -14497,7 +14514,7 @@
         <v>26</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="7" t="s">
@@ -14640,7 +14657,7 @@
         <v>26</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86" s="7" t="s">
@@ -14783,7 +14800,7 @@
         <v>28</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>29</v>
@@ -14962,7 +14979,7 @@
         <v>28</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="7" t="s">
@@ -15105,7 +15122,7 @@
         <v>28</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="7" t="s">
@@ -15248,7 +15265,7 @@
         <v>28</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="7" t="s">
@@ -15391,7 +15408,7 @@
         <v>28</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="7" t="s">
@@ -15534,7 +15551,7 @@
         <v>28</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="7" t="s">
@@ -15677,7 +15694,7 @@
         <v>28</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="7" t="s">
@@ -15820,7 +15837,7 @@
         <v>28</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C94" s="7"/>
       <c r="D94" s="7" t="s">
@@ -15960,13 +15977,13 @@
     </row>
     <row r="95" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="8">
@@ -16139,10 +16156,10 @@
     </row>
     <row r="96" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C96" s="7"/>
       <c r="D96" s="7" t="s">
@@ -16282,10 +16299,10 @@
     </row>
     <row r="97" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C97" s="7"/>
       <c r="D97" s="7" t="s">
@@ -16425,10 +16442,10 @@
     </row>
     <row r="98" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C98" s="7"/>
       <c r="D98" s="7" t="s">
@@ -16568,10 +16585,10 @@
     </row>
     <row r="99" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C99" s="7"/>
       <c r="D99" s="7" t="s">
@@ -16711,10 +16728,10 @@
     </row>
     <row r="100" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C100" s="7"/>
       <c r="D100" s="7" t="s">
@@ -16854,10 +16871,10 @@
     </row>
     <row r="101" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="7" t="s">
@@ -16997,10 +17014,10 @@
     </row>
     <row r="102" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C102" s="7"/>
       <c r="D102" s="7" t="s">
@@ -17143,7 +17160,7 @@
         <v>30</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>31</v>
@@ -17322,7 +17339,7 @@
         <v>30</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C104" s="7"/>
       <c r="D104" s="7" t="s">
@@ -17465,7 +17482,7 @@
         <v>30</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C105" s="7"/>
       <c r="D105" s="7" t="s">
@@ -17608,7 +17625,7 @@
         <v>30</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C106" s="7"/>
       <c r="D106" s="7" t="s">
@@ -17751,7 +17768,7 @@
         <v>30</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C107" s="7"/>
       <c r="D107" s="7" t="s">
@@ -17894,7 +17911,7 @@
         <v>30</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C108" s="7"/>
       <c r="D108" s="7" t="s">
@@ -18037,7 +18054,7 @@
         <v>30</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C109" s="7"/>
       <c r="D109" s="7" t="s">
@@ -18180,7 +18197,7 @@
         <v>30</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C110" s="7"/>
       <c r="D110" s="7" t="s">
@@ -18323,7 +18340,7 @@
         <v>32</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>33</v>
@@ -18502,7 +18519,7 @@
         <v>32</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C112" s="7"/>
       <c r="D112" s="7" t="s">
@@ -18645,7 +18662,7 @@
         <v>32</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C113" s="7"/>
       <c r="D113" s="7" t="s">
@@ -18788,7 +18805,7 @@
         <v>32</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C114" s="7"/>
       <c r="D114" s="7" t="s">
@@ -18931,7 +18948,7 @@
         <v>32</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C115" s="7"/>
       <c r="D115" s="7" t="s">
@@ -19074,7 +19091,7 @@
         <v>32</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C116" s="7"/>
       <c r="D116" s="7" t="s">
@@ -19217,7 +19234,7 @@
         <v>32</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C117" s="7"/>
       <c r="D117" s="7" t="s">
@@ -19360,7 +19377,7 @@
         <v>32</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C118" s="7"/>
       <c r="D118" s="7" t="s">
@@ -19503,7 +19520,7 @@
         <v>34</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>35</v>
@@ -19682,7 +19699,7 @@
         <v>34</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C120" s="7"/>
       <c r="D120" s="7" t="s">
@@ -19825,7 +19842,7 @@
         <v>34</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C121" s="7"/>
       <c r="D121" s="7" t="s">
@@ -19968,7 +19985,7 @@
         <v>34</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C122" s="7"/>
       <c r="D122" s="7" t="s">
@@ -20111,7 +20128,7 @@
         <v>34</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C123" s="7"/>
       <c r="D123" s="7" t="s">
@@ -20254,7 +20271,7 @@
         <v>34</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C124" s="7"/>
       <c r="D124" s="7" t="s">
@@ -20397,7 +20414,7 @@
         <v>34</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C125" s="7"/>
       <c r="D125" s="7" t="s">
@@ -20540,7 +20557,7 @@
         <v>34</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C126" s="7"/>
       <c r="D126" s="7" t="s">
@@ -20683,7 +20700,7 @@
         <v>53</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>36</v>
@@ -20862,7 +20879,7 @@
         <v>53</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C128" s="7"/>
       <c r="D128" s="7" t="s">
@@ -21005,7 +21022,7 @@
         <v>53</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C129" s="7"/>
       <c r="D129" s="7" t="s">
@@ -21148,7 +21165,7 @@
         <v>53</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C130" s="7"/>
       <c r="D130" s="7" t="s">
@@ -21291,7 +21308,7 @@
         <v>53</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C131" s="7"/>
       <c r="D131" s="7" t="s">
@@ -21434,7 +21451,7 @@
         <v>53</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C132" s="7"/>
       <c r="D132" s="7" t="s">
@@ -21577,7 +21594,7 @@
         <v>53</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C133" s="7"/>
       <c r="D133" s="7" t="s">
@@ -21720,7 +21737,7 @@
         <v>53</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C134" s="7"/>
       <c r="D134" s="7" t="s">
@@ -21863,7 +21880,7 @@
         <v>37</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>38</v>
@@ -22042,7 +22059,7 @@
         <v>37</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C136" s="7"/>
       <c r="D136" s="7" t="s">
@@ -22185,7 +22202,7 @@
         <v>37</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C137" s="7"/>
       <c r="D137" s="7" t="s">
@@ -22328,7 +22345,7 @@
         <v>37</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C138" s="7"/>
       <c r="D138" s="7" t="s">
@@ -22471,7 +22488,7 @@
         <v>37</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C139" s="7"/>
       <c r="D139" s="7" t="s">
@@ -22614,7 +22631,7 @@
         <v>37</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C140" s="7"/>
       <c r="D140" s="7" t="s">
@@ -22757,7 +22774,7 @@
         <v>37</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C141" s="7"/>
       <c r="D141" s="7" t="s">
@@ -22900,7 +22917,7 @@
         <v>37</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C142" s="7"/>
       <c r="D142" s="7" t="s">
@@ -23043,7 +23060,7 @@
         <v>39</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>39</v>
@@ -23222,7 +23239,7 @@
         <v>39</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C144" s="7"/>
       <c r="D144" s="7" t="s">
@@ -23365,7 +23382,7 @@
         <v>39</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C145" s="7"/>
       <c r="D145" s="7" t="s">
@@ -23508,7 +23525,7 @@
         <v>39</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C146" s="7"/>
       <c r="D146" s="7" t="s">
@@ -23651,7 +23668,7 @@
         <v>39</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C147" s="7"/>
       <c r="D147" s="7" t="s">
@@ -23794,7 +23811,7 @@
         <v>39</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C148" s="7"/>
       <c r="D148" s="7" t="s">
@@ -23937,7 +23954,7 @@
         <v>39</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C149" s="7"/>
       <c r="D149" s="7" t="s">
@@ -24080,7 +24097,7 @@
         <v>39</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C150" s="7"/>
       <c r="D150" s="7" t="s">
@@ -24223,7 +24240,7 @@
         <v>40</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C151" s="7" t="s">
         <v>40</v>
@@ -24402,7 +24419,7 @@
         <v>40</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C152" s="7"/>
       <c r="D152" s="7" t="s">
@@ -24545,7 +24562,7 @@
         <v>40</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C153" s="7"/>
       <c r="D153" s="7" t="s">
@@ -24688,7 +24705,7 @@
         <v>40</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C154" s="7"/>
       <c r="D154" s="7" t="s">
@@ -24831,7 +24848,7 @@
         <v>40</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C155" s="7"/>
       <c r="D155" s="7" t="s">
@@ -24974,7 +24991,7 @@
         <v>40</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C156" s="7"/>
       <c r="D156" s="7" t="s">
@@ -25117,7 +25134,7 @@
         <v>40</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C157" s="7"/>
       <c r="D157" s="7" t="s">
@@ -25260,7 +25277,7 @@
         <v>40</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C158" s="7"/>
       <c r="D158" s="7" t="s">
@@ -25403,7 +25420,7 @@
         <v>41</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C159" s="7" t="s">
         <v>41</v>
@@ -25582,7 +25599,7 @@
         <v>41</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C160" s="7"/>
       <c r="D160" s="7" t="s">
@@ -25725,7 +25742,7 @@
         <v>41</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C161" s="7"/>
       <c r="D161" s="7" t="s">
@@ -25868,7 +25885,7 @@
         <v>41</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C162" s="7"/>
       <c r="D162" s="7" t="s">
@@ -26011,7 +26028,7 @@
         <v>41</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C163" s="7"/>
       <c r="D163" s="7" t="s">
@@ -26154,7 +26171,7 @@
         <v>41</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C164" s="7"/>
       <c r="D164" s="7" t="s">
@@ -26297,7 +26314,7 @@
         <v>41</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C165" s="7"/>
       <c r="D165" s="7" t="s">
@@ -26440,7 +26457,7 @@
         <v>41</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C166" s="7"/>
       <c r="D166" s="7" t="s">
@@ -28943,7 +28960,7 @@
         <v>44</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C183" s="7" t="s">
         <v>44</v>
@@ -29122,7 +29139,7 @@
         <v>44</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C184" s="7"/>
       <c r="D184" s="7" t="s">
@@ -29265,7 +29282,7 @@
         <v>44</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C185" s="7"/>
       <c r="D185" s="7" t="s">
@@ -29408,7 +29425,7 @@
         <v>44</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C186" s="7"/>
       <c r="D186" s="7" t="s">
@@ -29551,7 +29568,7 @@
         <v>44</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C187" s="7"/>
       <c r="D187" s="7" t="s">
@@ -29694,7 +29711,7 @@
         <v>44</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C188" s="7"/>
       <c r="D188" s="7" t="s">
@@ -29837,7 +29854,7 @@
         <v>44</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C189" s="7"/>
       <c r="D189" s="7" t="s">
@@ -29980,7 +29997,7 @@
         <v>44</v>
       </c>
       <c r="B190" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C190" s="7"/>
       <c r="D190" s="7" t="s">
@@ -30123,7 +30140,7 @@
         <v>44</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C191" s="7" t="s">
         <v>45</v>
@@ -30302,7 +30319,7 @@
         <v>46</v>
       </c>
       <c r="B192" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C192" s="7"/>
       <c r="D192" s="7" t="s">
@@ -30445,7 +30462,7 @@
         <v>46</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C193" s="7"/>
       <c r="D193" s="7" t="s">
@@ -30588,7 +30605,7 @@
         <v>46</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C194" s="7"/>
       <c r="D194" s="7" t="s">
@@ -30731,7 +30748,7 @@
         <v>46</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C195" s="7"/>
       <c r="D195" s="7" t="s">
@@ -30874,7 +30891,7 @@
         <v>46</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C196" s="7"/>
       <c r="D196" s="7" t="s">
@@ -31017,7 +31034,7 @@
         <v>46</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C197" s="7"/>
       <c r="D197" s="7" t="s">
@@ -31160,7 +31177,7 @@
         <v>46</v>
       </c>
       <c r="B198" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C198" s="7"/>
       <c r="D198" s="7" t="s">
@@ -31344,12 +31361,13 @@
     </row>
   </sheetData>
   <autoFilter ref="B4:W198" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <sortState ref="D6:D12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D6:D12">
     <sortCondition ref="D6"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="G3:J3"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update templete 2025 ni Bos Senggol dong
</commit_message>
<xml_diff>
--- a/public/files/TemplateCapexExport.xlsx
+++ b/public/files/TemplateCapexExport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Project Management\01_Source code\new_cubic_pro\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fabian\00_Project\cubic_pro\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5884BFC0-31F4-4773-AF64-70BD560EBB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96398CF-ECFB-4A24-B375-E2206387A190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary CAPEX" sheetId="3" r:id="rId1"/>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Dept</t>
-  </si>
-  <si>
-    <t>FY 2024</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -282,6 +279,9 @@
   <si>
     <t>HRG2</t>
   </si>
+  <si>
+    <t>FY 2025</t>
+  </si>
 </sst>
 </file>
 
@@ -433,11 +433,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Koma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Persen" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -718,10 +718,10 @@
   <dimension ref="A3:AT14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="X5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -735,7 +735,9 @@
     <col min="9" max="9" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="17" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.453125" customWidth="1"/>
+    <col min="15" max="17" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="8.453125" bestFit="1" customWidth="1"/>
@@ -754,251 +756,251 @@
     <row r="3" spans="1:46" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="13" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
       <c r="I3" s="2">
-        <v>45383</v>
+        <v>45748</v>
       </c>
       <c r="J3" s="2">
-        <v>45413</v>
+        <v>45778</v>
       </c>
       <c r="K3" s="2">
-        <v>45444</v>
+        <v>45809</v>
       </c>
       <c r="L3" s="2">
-        <v>45474</v>
+        <v>45839</v>
       </c>
       <c r="M3" s="2">
-        <v>45505</v>
+        <v>45870</v>
       </c>
       <c r="N3" s="2">
-        <v>45536</v>
+        <v>45901</v>
       </c>
       <c r="O3" s="2">
-        <v>45566</v>
+        <v>45931</v>
       </c>
       <c r="P3" s="2">
-        <v>45597</v>
+        <v>45962</v>
       </c>
       <c r="Q3" s="2">
-        <v>45627</v>
+        <v>45992</v>
       </c>
       <c r="R3" s="2">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="S3" s="2">
-        <v>45689</v>
+        <v>46054</v>
       </c>
       <c r="T3" s="2">
-        <v>45717</v>
+        <v>46082</v>
       </c>
       <c r="U3" s="1"/>
       <c r="V3" s="2">
-        <v>45383</v>
+        <v>45748</v>
       </c>
       <c r="W3" s="2">
-        <v>45413</v>
+        <v>45778</v>
       </c>
       <c r="X3" s="2">
-        <v>45444</v>
+        <v>45809</v>
       </c>
       <c r="Y3" s="2">
-        <v>45474</v>
+        <v>45839</v>
       </c>
       <c r="Z3" s="2">
-        <v>45505</v>
+        <v>45870</v>
       </c>
       <c r="AA3" s="2">
-        <v>45536</v>
+        <v>45901</v>
       </c>
       <c r="AB3" s="2">
-        <v>45566</v>
+        <v>45931</v>
       </c>
       <c r="AC3" s="2">
-        <v>45597</v>
+        <v>45962</v>
       </c>
       <c r="AD3" s="2">
-        <v>45627</v>
+        <v>45992</v>
       </c>
       <c r="AE3" s="2">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="AF3" s="2">
-        <v>45689</v>
+        <v>46054</v>
       </c>
       <c r="AG3" s="2">
-        <v>45717</v>
+        <v>46082</v>
       </c>
       <c r="AI3" s="2">
-        <v>45383</v>
+        <v>45748</v>
       </c>
       <c r="AJ3" s="2">
-        <v>45413</v>
+        <v>45778</v>
       </c>
       <c r="AK3" s="2">
-        <v>45444</v>
+        <v>45809</v>
       </c>
       <c r="AL3" s="2">
-        <v>45474</v>
+        <v>45839</v>
       </c>
       <c r="AM3" s="2">
-        <v>45505</v>
+        <v>45870</v>
       </c>
       <c r="AN3" s="2">
-        <v>45536</v>
+        <v>45901</v>
       </c>
       <c r="AO3" s="2">
-        <v>45566</v>
+        <v>45931</v>
       </c>
       <c r="AP3" s="2">
-        <v>45597</v>
+        <v>45962</v>
       </c>
       <c r="AQ3" s="2">
-        <v>45627</v>
+        <v>45992</v>
       </c>
       <c r="AR3" s="2">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="AS3" s="2">
-        <v>45689</v>
+        <v>46054</v>
       </c>
       <c r="AT3" s="2">
-        <v>45717</v>
+        <v>46082</v>
       </c>
     </row>
     <row r="4" spans="1:46" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="AJ4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AK4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AL4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AM4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AN4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AO4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AP4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AQ4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AR4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AS4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AT4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:46" ht="15.5" x14ac:dyDescent="0.35">
@@ -1341,7 +1343,7 @@
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="8">
         <f t="shared" ref="B7:B13" si="47">G7</f>
@@ -1477,7 +1479,7 @@
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="8">
         <f t="shared" si="47"/>
@@ -1613,7 +1615,7 @@
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="8">
         <f t="shared" si="47"/>
@@ -1749,7 +1751,7 @@
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="8">
         <f t="shared" si="47"/>
@@ -1885,7 +1887,7 @@
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="8">
         <f t="shared" si="47"/>
@@ -2021,7 +2023,7 @@
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="8">
         <f t="shared" si="47"/>
@@ -2157,7 +2159,7 @@
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="8">
         <f t="shared" si="47"/>
@@ -2350,10 +2352,10 @@
   <dimension ref="A3:AW198"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="AH5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C148" sqref="C148"/>
+      <selection pane="bottomRight" activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2390,122 +2392,122 @@
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="13" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
       <c r="L3" s="2">
-        <v>45383</v>
+        <v>45748</v>
       </c>
       <c r="M3" s="2">
-        <v>45413</v>
+        <v>45778</v>
       </c>
       <c r="N3" s="2">
-        <v>45444</v>
+        <v>45809</v>
       </c>
       <c r="O3" s="2">
-        <v>45474</v>
+        <v>45839</v>
       </c>
       <c r="P3" s="2">
-        <v>45505</v>
+        <v>45870</v>
       </c>
       <c r="Q3" s="2">
-        <v>45536</v>
+        <v>45901</v>
       </c>
       <c r="R3" s="2">
-        <v>45566</v>
+        <v>45931</v>
       </c>
       <c r="S3" s="2">
-        <v>45597</v>
+        <v>45962</v>
       </c>
       <c r="T3" s="2">
-        <v>45627</v>
+        <v>45992</v>
       </c>
       <c r="U3" s="2">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="V3" s="2">
-        <v>45689</v>
+        <v>46054</v>
       </c>
       <c r="W3" s="2">
-        <v>45717</v>
+        <v>46082</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="2">
-        <v>45383</v>
+        <v>45748</v>
       </c>
       <c r="Z3" s="2">
-        <v>45413</v>
+        <v>45778</v>
       </c>
       <c r="AA3" s="2">
-        <v>45444</v>
+        <v>45809</v>
       </c>
       <c r="AB3" s="2">
-        <v>45474</v>
+        <v>45839</v>
       </c>
       <c r="AC3" s="2">
-        <v>45505</v>
+        <v>45870</v>
       </c>
       <c r="AD3" s="2">
-        <v>45536</v>
+        <v>45901</v>
       </c>
       <c r="AE3" s="2">
-        <v>45566</v>
+        <v>45931</v>
       </c>
       <c r="AF3" s="2">
-        <v>45597</v>
+        <v>45962</v>
       </c>
       <c r="AG3" s="2">
-        <v>45627</v>
+        <v>45992</v>
       </c>
       <c r="AH3" s="2">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="AI3" s="2">
-        <v>45689</v>
+        <v>46054</v>
       </c>
       <c r="AJ3" s="2">
-        <v>45717</v>
+        <v>46082</v>
       </c>
       <c r="AL3" s="2">
-        <v>45383</v>
+        <v>45748</v>
       </c>
       <c r="AM3" s="2">
-        <v>45413</v>
+        <v>45778</v>
       </c>
       <c r="AN3" s="2">
-        <v>45444</v>
+        <v>45809</v>
       </c>
       <c r="AO3" s="2">
-        <v>45474</v>
+        <v>45839</v>
       </c>
       <c r="AP3" s="2">
-        <v>45505</v>
+        <v>45870</v>
       </c>
       <c r="AQ3" s="2">
-        <v>45536</v>
+        <v>45901</v>
       </c>
       <c r="AR3" s="2">
-        <v>45566</v>
+        <v>45931</v>
       </c>
       <c r="AS3" s="2">
-        <v>45597</v>
+        <v>45962</v>
       </c>
       <c r="AT3" s="2">
-        <v>45627</v>
+        <v>45992</v>
       </c>
       <c r="AU3" s="2">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="AV3" s="2">
-        <v>45689</v>
+        <v>46054</v>
       </c>
       <c r="AW3" s="2">
-        <v>45717</v>
+        <v>46082</v>
       </c>
     </row>
     <row r="4" spans="1:49" ht="31" x14ac:dyDescent="0.35">
@@ -2516,314 +2518,314 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="AM4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AN4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AO4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AP4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AQ4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AR4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AS4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AT4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AU4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AV4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AW4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:49" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="12" t="e">
-        <f>(SUM(E6:E197)/2)-#REF!</f>
-        <v>#REF!</v>
+      <c r="E5" s="12">
+        <f>(SUM(E6:E197)/2)</f>
+        <v>0</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="12" t="e">
-        <f>(SUM(G6:G197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H5" s="12" t="e">
-        <f>(SUM(H6:H197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I5" s="12" t="e">
-        <f>(SUM(I6:I197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J5" s="12" t="e">
-        <f>(SUM(J6:J197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L5" s="12" t="e">
-        <f>(SUM(L6:L197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M5" s="12" t="e">
-        <f>(SUM(M6:M197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N5" s="12" t="e">
-        <f>(SUM(N6:N197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O5" s="12" t="e">
-        <f>(SUM(O6:O197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P5" s="12" t="e">
-        <f>(SUM(P6:P197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q5" s="12" t="e">
-        <f>(SUM(Q6:Q197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R5" s="12" t="e">
-        <f>(SUM(R6:R197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S5" s="12" t="e">
-        <f>(SUM(S6:S197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T5" s="12" t="e">
-        <f>(SUM(T6:T197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="U5" s="12" t="e">
-        <f>(SUM(U6:U197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V5" s="12" t="e">
-        <f>(SUM(V6:V197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W5" s="12" t="e">
-        <f>(SUM(W6:W197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Y5" s="12" t="e">
-        <f>(SUM(Y6:Y197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Z5" s="12" t="e">
-        <f>(SUM(Z6:Z197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AA5" s="12" t="e">
-        <f>(SUM(AA6:AA197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AB5" s="12" t="e">
-        <f>(SUM(AB6:AB197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AC5" s="12" t="e">
-        <f>(SUM(AC6:AC197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AD5" s="12" t="e">
-        <f>(SUM(AD6:AD197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AE5" s="12" t="e">
-        <f>(SUM(AE6:AE197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AF5" s="12" t="e">
-        <f>(SUM(AF6:AF197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AG5" s="12" t="e">
-        <f>(SUM(AG6:AG197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AH5" s="12" t="e">
-        <f>(SUM(AH6:AH197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AI5" s="12" t="e">
-        <f>(SUM(AI6:AI197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AJ5" s="12" t="e">
-        <f>(SUM(AJ6:AJ197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AL5" s="12" t="e">
-        <f>(SUM(AL6:AL197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AM5" s="12" t="e">
-        <f>(SUM(AM6:AM197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AN5" s="12" t="e">
-        <f>(SUM(AN6:AN197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AO5" s="12" t="e">
-        <f>(SUM(AO6:AO197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AP5" s="12" t="e">
-        <f>(SUM(AP6:AP197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AQ5" s="12" t="e">
-        <f>(SUM(AQ6:AQ197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AR5" s="12" t="e">
-        <f>(SUM(AR6:AR197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AS5" s="12" t="e">
-        <f>(SUM(AS6:AS197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AT5" s="12" t="e">
-        <f>(SUM(AT6:AT197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AU5" s="12" t="e">
-        <f>(SUM(AU6:AU197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AV5" s="12" t="e">
-        <f>(SUM(AV6:AV197)/2)-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AW5" s="12" t="e">
-        <f>(SUM(AW6:AW197)/2)-#REF!</f>
-        <v>#REF!</v>
+      <c r="G5" s="12">
+        <f>(SUM(G6:G197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="12">
+        <f>(SUM(H6:H197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="12">
+        <f>(SUM(I6:I197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="12">
+        <f>(SUM(J6:J197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
+        <f>(SUM(L6:L197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="12">
+        <f>(SUM(M6:M197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="12">
+        <f>(SUM(N6:N197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="12">
+        <f>(SUM(O6:O197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="12">
+        <f>(SUM(P6:P197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="12">
+        <f>(SUM(Q6:Q197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="12">
+        <f>(SUM(R6:R197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="12">
+        <f>(SUM(S6:S197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="12">
+        <f>(SUM(T6:T197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="12">
+        <f>(SUM(U6:U197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="12">
+        <f>(SUM(V6:V197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="12">
+        <f>(SUM(W6:W197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="12">
+        <f>(SUM(Y6:Y197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="12">
+        <f>(SUM(Z6:Z197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="12">
+        <f>(SUM(AA6:AA197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="12">
+        <f>(SUM(AB6:AB197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="12">
+        <f>(SUM(AC6:AC197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AD5" s="12">
+        <f>(SUM(AD6:AD197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AE5" s="12">
+        <f>(SUM(AE6:AE197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="12">
+        <f>(SUM(AF6:AF197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AG5" s="12">
+        <f>(SUM(AG6:AG197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="12">
+        <f>(SUM(AH6:AH197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AI5" s="12">
+        <f>(SUM(AI6:AI197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="12">
+        <f>(SUM(AJ6:AJ197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AL5" s="12">
+        <f>(SUM(AL6:AL197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AM5" s="12">
+        <f>(SUM(AM6:AM197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AN5" s="12">
+        <f>(SUM(AN6:AN197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AO5" s="12">
+        <f>(SUM(AO6:AO197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AP5" s="12">
+        <f>(SUM(AP6:AP197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="12">
+        <f>(SUM(AQ6:AQ197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AR5" s="12">
+        <f>(SUM(AR6:AR197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AS5" s="12">
+        <f>(SUM(AS6:AS197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AT5" s="12">
+        <f>(SUM(AT6:AT197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AU5" s="12">
+        <f>(SUM(AU6:AU197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AV5" s="12">
+        <f>(SUM(AV6:AV197)/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AW5" s="12">
+        <f>(SUM(AW6:AW197)/2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8">
@@ -2996,14 +2998,14 @@
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="8">
         <f t="shared" ref="E7:E69" si="4">J7</f>
@@ -3139,14 +3141,14 @@
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="8">
         <f t="shared" si="4"/>
@@ -3282,14 +3284,14 @@
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="8">
         <f t="shared" si="4"/>
@@ -3425,14 +3427,14 @@
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="8">
         <f t="shared" si="4"/>
@@ -3568,14 +3570,14 @@
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="8">
         <f t="shared" si="4"/>
@@ -3711,14 +3713,14 @@
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="8">
         <f t="shared" si="4"/>
@@ -3854,14 +3856,14 @@
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="8">
         <f t="shared" si="4"/>
@@ -3997,13 +3999,13 @@
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8">
@@ -4176,14 +4178,14 @@
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="8">
         <f t="shared" si="4"/>
@@ -4319,14 +4321,14 @@
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="8">
         <f t="shared" si="4"/>
@@ -4462,14 +4464,14 @@
     </row>
     <row r="17" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="8">
         <f t="shared" si="4"/>
@@ -4605,14 +4607,14 @@
     </row>
     <row r="18" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="8">
         <f t="shared" si="4"/>
@@ -4748,14 +4750,14 @@
     </row>
     <row r="19" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" s="8">
         <f t="shared" si="4"/>
@@ -4891,14 +4893,14 @@
     </row>
     <row r="20" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" s="8">
         <f t="shared" si="4"/>
@@ -5034,14 +5036,14 @@
     </row>
     <row r="21" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" s="8">
         <f t="shared" si="4"/>
@@ -5177,13 +5179,13 @@
     </row>
     <row r="22" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="8">
@@ -5356,14 +5358,14 @@
     </row>
     <row r="23" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" s="8">
         <f t="shared" si="4"/>
@@ -5499,14 +5501,14 @@
     </row>
     <row r="24" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" s="8">
         <f t="shared" si="4"/>
@@ -5642,14 +5644,14 @@
     </row>
     <row r="25" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="8">
         <f t="shared" si="4"/>
@@ -5785,14 +5787,14 @@
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" s="8">
         <f t="shared" si="4"/>
@@ -5928,14 +5930,14 @@
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E27" s="8">
         <f t="shared" si="4"/>
@@ -6071,14 +6073,14 @@
     </row>
     <row r="28" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28" s="8">
         <f t="shared" si="4"/>
@@ -6214,14 +6216,14 @@
     </row>
     <row r="29" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E29" s="8">
         <f t="shared" si="4"/>
@@ -6357,13 +6359,13 @@
     </row>
     <row r="30" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="8">
@@ -6536,14 +6538,14 @@
     </row>
     <row r="31" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E31" s="8">
         <f t="shared" si="4"/>
@@ -6679,14 +6681,14 @@
     </row>
     <row r="32" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E32" s="8">
         <f t="shared" si="4"/>
@@ -6822,14 +6824,14 @@
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33" s="8">
         <f t="shared" si="4"/>
@@ -6965,14 +6967,14 @@
     </row>
     <row r="34" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E34" s="8">
         <f t="shared" si="4"/>
@@ -7108,14 +7110,14 @@
     </row>
     <row r="35" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E35" s="8">
         <f t="shared" si="4"/>
@@ -7251,14 +7253,14 @@
     </row>
     <row r="36" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E36" s="8">
         <f t="shared" si="4"/>
@@ -7394,14 +7396,14 @@
     </row>
     <row r="37" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E37" s="8">
         <f t="shared" si="4"/>
@@ -7537,13 +7539,13 @@
     </row>
     <row r="38" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="8">
@@ -7716,14 +7718,14 @@
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E39" s="8">
         <f t="shared" si="4"/>
@@ -7859,14 +7861,14 @@
     </row>
     <row r="40" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40" s="8">
         <f t="shared" si="4"/>
@@ -8002,14 +8004,14 @@
     </row>
     <row r="41" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E41" s="8">
         <f t="shared" si="4"/>
@@ -8145,14 +8147,14 @@
     </row>
     <row r="42" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E42" s="8">
         <f t="shared" si="4"/>
@@ -8288,14 +8290,14 @@
     </row>
     <row r="43" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E43" s="8">
         <f t="shared" si="4"/>
@@ -8431,14 +8433,14 @@
     </row>
     <row r="44" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E44" s="8">
         <f t="shared" si="4"/>
@@ -8574,14 +8576,14 @@
     </row>
     <row r="45" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E45" s="8">
         <f t="shared" si="4"/>
@@ -8717,13 +8719,13 @@
     </row>
     <row r="46" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="8">
@@ -8896,14 +8898,14 @@
     </row>
     <row r="47" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E47" s="8">
         <f t="shared" si="4"/>
@@ -9039,14 +9041,14 @@
     </row>
     <row r="48" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E48" s="8">
         <f t="shared" si="4"/>
@@ -9182,14 +9184,14 @@
     </row>
     <row r="49" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E49" s="8">
         <f t="shared" si="4"/>
@@ -9325,14 +9327,14 @@
     </row>
     <row r="50" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E50" s="8">
         <f t="shared" si="4"/>
@@ -9468,14 +9470,14 @@
     </row>
     <row r="51" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E51" s="8">
         <f t="shared" si="4"/>
@@ -9611,14 +9613,14 @@
     </row>
     <row r="52" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E52" s="8">
         <f t="shared" si="4"/>
@@ -9754,14 +9756,14 @@
     </row>
     <row r="53" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E53" s="8">
         <f t="shared" si="4"/>
@@ -9897,13 +9899,13 @@
     </row>
     <row r="54" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="8">
@@ -10076,14 +10078,14 @@
     </row>
     <row r="55" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E55" s="8">
         <f t="shared" si="4"/>
@@ -10219,14 +10221,14 @@
     </row>
     <row r="56" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E56" s="8">
         <f t="shared" si="4"/>
@@ -10362,14 +10364,14 @@
     </row>
     <row r="57" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E57" s="8">
         <f t="shared" si="4"/>
@@ -10505,14 +10507,14 @@
     </row>
     <row r="58" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E58" s="8">
         <f t="shared" si="4"/>
@@ -10648,14 +10650,14 @@
     </row>
     <row r="59" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E59" s="8">
         <f t="shared" si="4"/>
@@ -10791,14 +10793,14 @@
     </row>
     <row r="60" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E60" s="8">
         <f t="shared" si="4"/>
@@ -10934,14 +10936,14 @@
     </row>
     <row r="61" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E61" s="8">
         <f t="shared" si="4"/>
@@ -11077,13 +11079,13 @@
     </row>
     <row r="62" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="8">
@@ -11256,14 +11258,14 @@
     </row>
     <row r="63" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E63" s="8">
         <f t="shared" si="4"/>
@@ -11399,14 +11401,14 @@
     </row>
     <row r="64" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E64" s="8">
         <f t="shared" si="4"/>
@@ -11542,14 +11544,14 @@
     </row>
     <row r="65" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E65" s="8">
         <f t="shared" si="4"/>
@@ -11685,14 +11687,14 @@
     </row>
     <row r="66" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E66" s="8">
         <f t="shared" si="4"/>
@@ -11828,14 +11830,14 @@
     </row>
     <row r="67" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E67" s="8">
         <f t="shared" si="4"/>
@@ -11971,14 +11973,14 @@
     </row>
     <row r="68" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E68" s="8">
         <f t="shared" si="4"/>
@@ -12114,14 +12116,14 @@
     </row>
     <row r="69" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E69" s="8">
         <f t="shared" si="4"/>
@@ -12257,13 +12259,13 @@
     </row>
     <row r="70" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="8">
@@ -12436,14 +12438,14 @@
     </row>
     <row r="71" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E71" s="8">
         <f t="shared" ref="E71:E141" si="158">J71</f>
@@ -12579,14 +12581,14 @@
     </row>
     <row r="72" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C72" s="7"/>
       <c r="D72" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E72" s="8">
         <f t="shared" si="158"/>
@@ -12722,14 +12724,14 @@
     </row>
     <row r="73" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E73" s="8">
         <f t="shared" si="158"/>
@@ -12865,14 +12867,14 @@
     </row>
     <row r="74" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C74" s="7"/>
       <c r="D74" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E74" s="8">
         <f t="shared" si="158"/>
@@ -13008,14 +13010,14 @@
     </row>
     <row r="75" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E75" s="8">
         <f t="shared" si="158"/>
@@ -13151,14 +13153,14 @@
     </row>
     <row r="76" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C76" s="7"/>
       <c r="D76" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E76" s="8">
         <f t="shared" si="158"/>
@@ -13294,14 +13296,14 @@
     </row>
     <row r="77" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E77" s="8">
         <f t="shared" si="158"/>
@@ -13437,13 +13439,13 @@
     </row>
     <row r="78" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>23</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="8">
@@ -13616,14 +13618,14 @@
     </row>
     <row r="79" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E79" s="8">
         <f t="shared" si="158"/>
@@ -13759,14 +13761,14 @@
     </row>
     <row r="80" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E80" s="8">
         <f t="shared" si="158"/>
@@ -13902,14 +13904,14 @@
     </row>
     <row r="81" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C81" s="7"/>
       <c r="D81" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E81" s="8">
         <f t="shared" si="158"/>
@@ -14045,14 +14047,14 @@
     </row>
     <row r="82" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C82" s="7"/>
       <c r="D82" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E82" s="8">
         <f t="shared" si="158"/>
@@ -14188,14 +14190,14 @@
     </row>
     <row r="83" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E83" s="8">
         <f t="shared" si="158"/>
@@ -14331,14 +14333,14 @@
     </row>
     <row r="84" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C84" s="7"/>
       <c r="D84" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E84" s="8">
         <f t="shared" si="158"/>
@@ -14474,14 +14476,14 @@
     </row>
     <row r="85" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E85" s="8">
         <f t="shared" si="158"/>
@@ -14617,13 +14619,13 @@
     </row>
     <row r="86" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C86" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="8">
@@ -14796,14 +14798,14 @@
     </row>
     <row r="87" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E87" s="8">
         <f t="shared" si="158"/>
@@ -14939,14 +14941,14 @@
     </row>
     <row r="88" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E88" s="8">
         <f t="shared" si="158"/>
@@ -15082,14 +15084,14 @@
     </row>
     <row r="89" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E89" s="8">
         <f t="shared" si="158"/>
@@ -15225,14 +15227,14 @@
     </row>
     <row r="90" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E90" s="8">
         <f t="shared" si="158"/>
@@ -15368,14 +15370,14 @@
     </row>
     <row r="91" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E91" s="8">
         <f t="shared" si="158"/>
@@ -15511,14 +15513,14 @@
     </row>
     <row r="92" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E92" s="8">
         <f t="shared" si="158"/>
@@ -15654,14 +15656,14 @@
     </row>
     <row r="93" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E93" s="8">
         <f t="shared" si="158"/>
@@ -15797,13 +15799,13 @@
     </row>
     <row r="94" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="8">
@@ -15976,14 +15978,14 @@
     </row>
     <row r="95" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E95" s="8">
         <f t="shared" ref="E95:E101" si="204">J95</f>
@@ -16119,14 +16121,14 @@
     </row>
     <row r="96" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C96" s="7"/>
       <c r="D96" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E96" s="8">
         <f t="shared" si="204"/>
@@ -16262,14 +16264,14 @@
     </row>
     <row r="97" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C97" s="7"/>
       <c r="D97" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E97" s="8">
         <f t="shared" si="204"/>
@@ -16405,14 +16407,14 @@
     </row>
     <row r="98" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C98" s="7"/>
       <c r="D98" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E98" s="8">
         <f t="shared" si="204"/>
@@ -16548,14 +16550,14 @@
     </row>
     <row r="99" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C99" s="7"/>
       <c r="D99" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E99" s="8">
         <f t="shared" si="204"/>
@@ -16691,14 +16693,14 @@
     </row>
     <row r="100" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C100" s="7"/>
       <c r="D100" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E100" s="8">
         <f t="shared" si="204"/>
@@ -16834,14 +16836,14 @@
     </row>
     <row r="101" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E101" s="8">
         <f t="shared" si="204"/>
@@ -16977,13 +16979,13 @@
     </row>
     <row r="102" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
+        <v>27</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C102" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="8">
@@ -17156,14 +17158,14 @@
     </row>
     <row r="103" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C103" s="7"/>
       <c r="D103" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E103" s="8">
         <f t="shared" si="158"/>
@@ -17299,14 +17301,14 @@
     </row>
     <row r="104" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C104" s="7"/>
       <c r="D104" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E104" s="8">
         <f t="shared" si="158"/>
@@ -17442,14 +17444,14 @@
     </row>
     <row r="105" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C105" s="7"/>
       <c r="D105" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E105" s="8">
         <f t="shared" si="158"/>
@@ -17585,14 +17587,14 @@
     </row>
     <row r="106" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C106" s="7"/>
       <c r="D106" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E106" s="8">
         <f t="shared" si="158"/>
@@ -17728,14 +17730,14 @@
     </row>
     <row r="107" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C107" s="7"/>
       <c r="D107" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E107" s="8">
         <f t="shared" si="158"/>
@@ -17871,14 +17873,14 @@
     </row>
     <row r="108" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C108" s="7"/>
       <c r="D108" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E108" s="8">
         <f t="shared" si="158"/>
@@ -18014,14 +18016,14 @@
     </row>
     <row r="109" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C109" s="7"/>
       <c r="D109" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E109" s="8">
         <f t="shared" si="158"/>
@@ -18157,13 +18159,13 @@
     </row>
     <row r="110" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
+        <v>29</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C110" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="D110" s="7"/>
       <c r="E110" s="8">
@@ -18336,14 +18338,14 @@
     </row>
     <row r="111" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C111" s="7"/>
       <c r="D111" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E111" s="8">
         <f t="shared" si="158"/>
@@ -18479,14 +18481,14 @@
     </row>
     <row r="112" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C112" s="7"/>
       <c r="D112" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E112" s="8">
         <f t="shared" si="158"/>
@@ -18622,14 +18624,14 @@
     </row>
     <row r="113" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C113" s="7"/>
       <c r="D113" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E113" s="8">
         <f t="shared" si="158"/>
@@ -18765,14 +18767,14 @@
     </row>
     <row r="114" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C114" s="7"/>
       <c r="D114" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E114" s="8">
         <f t="shared" si="158"/>
@@ -18908,14 +18910,14 @@
     </row>
     <row r="115" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C115" s="7"/>
       <c r="D115" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E115" s="8">
         <f t="shared" si="158"/>
@@ -19051,14 +19053,14 @@
     </row>
     <row r="116" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C116" s="7"/>
       <c r="D116" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E116" s="8">
         <f t="shared" si="158"/>
@@ -19194,14 +19196,14 @@
     </row>
     <row r="117" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C117" s="7"/>
       <c r="D117" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E117" s="8">
         <f t="shared" si="158"/>
@@ -19337,13 +19339,13 @@
     </row>
     <row r="118" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
+        <v>31</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C118" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B118" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C118" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="8">
@@ -19516,14 +19518,14 @@
     </row>
     <row r="119" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C119" s="7"/>
       <c r="D119" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E119" s="8">
         <f t="shared" si="158"/>
@@ -19659,14 +19661,14 @@
     </row>
     <row r="120" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C120" s="7"/>
       <c r="D120" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E120" s="8">
         <f t="shared" si="158"/>
@@ -19802,14 +19804,14 @@
     </row>
     <row r="121" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C121" s="7"/>
       <c r="D121" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E121" s="8">
         <f t="shared" si="158"/>
@@ -19945,14 +19947,14 @@
     </row>
     <row r="122" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C122" s="7"/>
       <c r="D122" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E122" s="8">
         <f t="shared" si="158"/>
@@ -20088,14 +20090,14 @@
     </row>
     <row r="123" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C123" s="7"/>
       <c r="D123" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E123" s="8">
         <f t="shared" si="158"/>
@@ -20231,14 +20233,14 @@
     </row>
     <row r="124" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C124" s="7"/>
       <c r="D124" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E124" s="8">
         <f t="shared" si="158"/>
@@ -20374,14 +20376,14 @@
     </row>
     <row r="125" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C125" s="7"/>
       <c r="D125" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E125" s="8">
         <f t="shared" si="158"/>
@@ -20517,13 +20519,13 @@
     </row>
     <row r="126" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D126" s="7"/>
       <c r="E126" s="8">
@@ -20696,14 +20698,14 @@
     </row>
     <row r="127" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C127" s="7"/>
       <c r="D127" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E127" s="8">
         <f t="shared" si="158"/>
@@ -20839,14 +20841,14 @@
     </row>
     <row r="128" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C128" s="7"/>
       <c r="D128" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E128" s="8">
         <f t="shared" si="158"/>
@@ -20982,14 +20984,14 @@
     </row>
     <row r="129" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C129" s="7"/>
       <c r="D129" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E129" s="8">
         <f t="shared" si="158"/>
@@ -21125,14 +21127,14 @@
     </row>
     <row r="130" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C130" s="7"/>
       <c r="D130" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E130" s="8">
         <f t="shared" si="158"/>
@@ -21268,14 +21270,14 @@
     </row>
     <row r="131" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C131" s="7"/>
       <c r="D131" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E131" s="8">
         <f t="shared" si="158"/>
@@ -21411,14 +21413,14 @@
     </row>
     <row r="132" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C132" s="7"/>
       <c r="D132" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E132" s="8">
         <f t="shared" si="158"/>
@@ -21554,14 +21556,14 @@
     </row>
     <row r="133" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C133" s="7"/>
       <c r="D133" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E133" s="8">
         <f t="shared" si="158"/>
@@ -21697,13 +21699,13 @@
     </row>
     <row r="134" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
+        <v>34</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C134" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="B134" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="8">
@@ -21876,14 +21878,14 @@
     </row>
     <row r="135" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C135" s="7"/>
       <c r="D135" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E135" s="8">
         <f t="shared" si="158"/>
@@ -22019,14 +22021,14 @@
     </row>
     <row r="136" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C136" s="7"/>
       <c r="D136" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E136" s="8">
         <f t="shared" si="158"/>
@@ -22162,14 +22164,14 @@
     </row>
     <row r="137" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C137" s="7"/>
       <c r="D137" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E137" s="8">
         <f t="shared" si="158"/>
@@ -22305,14 +22307,14 @@
     </row>
     <row r="138" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C138" s="7"/>
       <c r="D138" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E138" s="8">
         <f t="shared" si="158"/>
@@ -22448,14 +22450,14 @@
     </row>
     <row r="139" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C139" s="7"/>
       <c r="D139" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E139" s="8">
         <f t="shared" si="158"/>
@@ -22591,14 +22593,14 @@
     </row>
     <row r="140" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C140" s="7"/>
       <c r="D140" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E140" s="8">
         <f t="shared" si="158"/>
@@ -22734,14 +22736,14 @@
     </row>
     <row r="141" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C141" s="7"/>
       <c r="D141" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E141" s="8">
         <f t="shared" si="158"/>
@@ -22877,13 +22879,13 @@
     </row>
     <row r="142" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D142" s="7"/>
       <c r="E142" s="8">
@@ -23056,14 +23058,14 @@
     </row>
     <row r="143" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C143" s="7"/>
       <c r="D143" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E143" s="8">
         <f t="shared" ref="E143:E197" si="319">J143</f>
@@ -23199,14 +23201,14 @@
     </row>
     <row r="144" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C144" s="7"/>
       <c r="D144" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E144" s="8">
         <f t="shared" si="319"/>
@@ -23342,14 +23344,14 @@
     </row>
     <row r="145" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C145" s="7"/>
       <c r="D145" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E145" s="8">
         <f t="shared" si="319"/>
@@ -23485,14 +23487,14 @@
     </row>
     <row r="146" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C146" s="7"/>
       <c r="D146" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E146" s="8">
         <f t="shared" si="319"/>
@@ -23628,14 +23630,14 @@
     </row>
     <row r="147" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C147" s="7"/>
       <c r="D147" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E147" s="8">
         <f t="shared" si="319"/>
@@ -23771,14 +23773,14 @@
     </row>
     <row r="148" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C148" s="7"/>
       <c r="D148" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E148" s="8">
         <f t="shared" si="319"/>
@@ -23914,14 +23916,14 @@
     </row>
     <row r="149" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C149" s="7"/>
       <c r="D149" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E149" s="8">
         <f t="shared" si="319"/>
@@ -24057,13 +24059,13 @@
     </row>
     <row r="150" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D150" s="7"/>
       <c r="E150" s="8">
@@ -24236,14 +24238,14 @@
     </row>
     <row r="151" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C151" s="7"/>
       <c r="D151" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E151" s="8">
         <f t="shared" si="319"/>
@@ -24379,14 +24381,14 @@
     </row>
     <row r="152" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C152" s="7"/>
       <c r="D152" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E152" s="8">
         <f t="shared" si="319"/>
@@ -24522,14 +24524,14 @@
     </row>
     <row r="153" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C153" s="7"/>
       <c r="D153" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E153" s="8">
         <f t="shared" si="319"/>
@@ -24665,14 +24667,14 @@
     </row>
     <row r="154" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C154" s="7"/>
       <c r="D154" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E154" s="8">
         <f t="shared" si="319"/>
@@ -24808,14 +24810,14 @@
     </row>
     <row r="155" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C155" s="7"/>
       <c r="D155" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E155" s="8">
         <f t="shared" si="319"/>
@@ -24951,14 +24953,14 @@
     </row>
     <row r="156" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C156" s="7"/>
       <c r="D156" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E156" s="8">
         <f t="shared" si="319"/>
@@ -25094,14 +25096,14 @@
     </row>
     <row r="157" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C157" s="7"/>
       <c r="D157" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E157" s="8">
         <f t="shared" si="319"/>
@@ -25237,13 +25239,13 @@
     </row>
     <row r="158" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D158" s="7"/>
       <c r="E158" s="8">
@@ -25416,14 +25418,14 @@
     </row>
     <row r="159" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C159" s="7"/>
       <c r="D159" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E159" s="8">
         <f t="shared" si="319"/>
@@ -25559,14 +25561,14 @@
     </row>
     <row r="160" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C160" s="7"/>
       <c r="D160" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E160" s="8">
         <f t="shared" si="319"/>
@@ -25702,14 +25704,14 @@
     </row>
     <row r="161" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C161" s="7"/>
       <c r="D161" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E161" s="8">
         <f t="shared" si="319"/>
@@ -25845,14 +25847,14 @@
     </row>
     <row r="162" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C162" s="7"/>
       <c r="D162" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E162" s="8">
         <f t="shared" si="319"/>
@@ -25988,14 +25990,14 @@
     </row>
     <row r="163" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C163" s="7"/>
       <c r="D163" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E163" s="8">
         <f t="shared" si="319"/>
@@ -26131,14 +26133,14 @@
     </row>
     <row r="164" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C164" s="7"/>
       <c r="D164" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E164" s="8">
         <f t="shared" si="319"/>
@@ -26274,14 +26276,14 @@
     </row>
     <row r="165" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C165" s="7"/>
       <c r="D165" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E165" s="8">
         <f t="shared" si="319"/>
@@ -26417,13 +26419,13 @@
     </row>
     <row r="166" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C166" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D166" s="7"/>
       <c r="E166" s="8">
@@ -26596,14 +26598,14 @@
     </row>
     <row r="167" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C167" s="7"/>
       <c r="D167" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E167" s="8">
         <f t="shared" si="319"/>
@@ -26739,14 +26741,14 @@
     </row>
     <row r="168" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C168" s="7"/>
       <c r="D168" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E168" s="8">
         <f t="shared" si="319"/>
@@ -26882,14 +26884,14 @@
     </row>
     <row r="169" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C169" s="7"/>
       <c r="D169" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E169" s="8">
         <f t="shared" si="319"/>
@@ -27025,14 +27027,14 @@
     </row>
     <row r="170" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C170" s="7"/>
       <c r="D170" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E170" s="8">
         <f t="shared" si="319"/>
@@ -27168,14 +27170,14 @@
     </row>
     <row r="171" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C171" s="7"/>
       <c r="D171" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E171" s="8">
         <f t="shared" si="319"/>
@@ -27311,14 +27313,14 @@
     </row>
     <row r="172" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C172" s="7"/>
       <c r="D172" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E172" s="8">
         <f t="shared" si="319"/>
@@ -27454,14 +27456,14 @@
     </row>
     <row r="173" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C173" s="7"/>
       <c r="D173" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E173" s="8">
         <f t="shared" si="319"/>
@@ -27597,13 +27599,13 @@
     </row>
     <row r="174" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D174" s="7"/>
       <c r="E174" s="8">
@@ -27776,14 +27778,14 @@
     </row>
     <row r="175" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C175" s="7"/>
       <c r="D175" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E175" s="8">
         <f t="shared" si="319"/>
@@ -27919,14 +27921,14 @@
     </row>
     <row r="176" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C176" s="7"/>
       <c r="D176" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E176" s="8">
         <f t="shared" si="319"/>
@@ -28062,14 +28064,14 @@
     </row>
     <row r="177" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C177" s="7"/>
       <c r="D177" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E177" s="8">
         <f t="shared" si="319"/>
@@ -28205,14 +28207,14 @@
     </row>
     <row r="178" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C178" s="7"/>
       <c r="D178" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E178" s="8">
         <f t="shared" si="319"/>
@@ -28348,14 +28350,14 @@
     </row>
     <row r="179" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C179" s="7"/>
       <c r="D179" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E179" s="8">
         <f t="shared" si="319"/>
@@ -28491,14 +28493,14 @@
     </row>
     <row r="180" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C180" s="7"/>
       <c r="D180" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E180" s="8">
         <f t="shared" si="319"/>
@@ -28634,14 +28636,14 @@
     </row>
     <row r="181" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C181" s="7"/>
       <c r="D181" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E181" s="8">
         <f t="shared" si="319"/>
@@ -28777,13 +28779,13 @@
     </row>
     <row r="182" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C182" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D182" s="7"/>
       <c r="E182" s="8">
@@ -28956,14 +28958,14 @@
     </row>
     <row r="183" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C183" s="7"/>
       <c r="D183" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E183" s="8">
         <f t="shared" si="319"/>
@@ -29099,14 +29101,14 @@
     </row>
     <row r="184" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C184" s="7"/>
       <c r="D184" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E184" s="8">
         <f t="shared" si="319"/>
@@ -29242,14 +29244,14 @@
     </row>
     <row r="185" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C185" s="7"/>
       <c r="D185" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E185" s="8">
         <f t="shared" si="319"/>
@@ -29385,14 +29387,14 @@
     </row>
     <row r="186" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C186" s="7"/>
       <c r="D186" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E186" s="8">
         <f t="shared" si="319"/>
@@ -29528,14 +29530,14 @@
     </row>
     <row r="187" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C187" s="7"/>
       <c r="D187" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E187" s="8">
         <f t="shared" si="319"/>
@@ -29671,14 +29673,14 @@
     </row>
     <row r="188" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C188" s="7"/>
       <c r="D188" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E188" s="8">
         <f t="shared" si="319"/>
@@ -29814,14 +29816,14 @@
     </row>
     <row r="189" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C189" s="7"/>
       <c r="D189" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E189" s="8">
         <f t="shared" si="319"/>
@@ -29957,13 +29959,13 @@
     </row>
     <row r="190" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
+        <v>41</v>
+      </c>
+      <c r="B190" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C190" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="B190" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C190" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="D190" s="7"/>
       <c r="E190" s="8">
@@ -30136,14 +30138,14 @@
     </row>
     <row r="191" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C191" s="7"/>
       <c r="D191" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E191" s="8">
         <f t="shared" si="319"/>
@@ -30279,14 +30281,14 @@
     </row>
     <row r="192" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B192" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C192" s="7"/>
       <c r="D192" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E192" s="8">
         <f t="shared" si="319"/>
@@ -30422,14 +30424,14 @@
     </row>
     <row r="193" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C193" s="7"/>
       <c r="D193" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E193" s="8">
         <f t="shared" si="319"/>
@@ -30565,14 +30567,14 @@
     </row>
     <row r="194" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C194" s="7"/>
       <c r="D194" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E194" s="8">
         <f t="shared" si="319"/>
@@ -30708,14 +30710,14 @@
     </row>
     <row r="195" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C195" s="7"/>
       <c r="D195" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E195" s="8">
         <f t="shared" si="319"/>
@@ -30851,14 +30853,14 @@
     </row>
     <row r="196" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C196" s="7"/>
       <c r="D196" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E196" s="8">
         <f t="shared" si="319"/>
@@ -30994,14 +30996,14 @@
     </row>
     <row r="197" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C197" s="7"/>
       <c r="D197" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E197" s="8">
         <f t="shared" si="319"/>

</xml_diff>